<commit_message>
Update Data Area Report 091122
</commit_message>
<xml_diff>
--- a/Database Area untuk Report.xlsx
+++ b/Database Area untuk Report.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25629"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25726"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Masterdata\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\steven.nathanael\Documents\Python\Data\2. Master Data Git\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D36886EE-37B1-492E-B489-98D141F03275}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0E59C86B-CECE-4CD7-BBD0-2EC4BCA75DA7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10560" xr2:uid="{CB92B276-28E0-4829-B796-ADBF995E2FE3}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" xr2:uid="{CB92B276-28E0-4829-B796-ADBF995E2FE3}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -39,7 +39,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="284" uniqueCount="117">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="286" uniqueCount="118">
   <si>
     <t>City</t>
   </si>
@@ -390,6 +390,9 @@
   </si>
   <si>
     <t>North Maluku Province</t>
+  </si>
+  <si>
+    <t>Jakarta Raya</t>
   </si>
 </sst>
 </file>
@@ -479,8 +482,7 @@
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
@@ -488,6 +490,9 @@
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
   </cellXfs>
@@ -804,10 +809,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{904F3AA4-01F5-4399-A1EE-4BB38BAA3B9E}">
-  <dimension ref="A1:B105"/>
+  <dimension ref="A1:B107"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A81" zoomScale="55" zoomScaleNormal="55" workbookViewId="0">
-      <selection activeCell="B105" sqref="B105"/>
+    <sheetView tabSelected="1" topLeftCell="A82" zoomScale="55" zoomScaleNormal="55" workbookViewId="0">
+      <selection activeCell="A107" sqref="A107"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -865,7 +870,7 @@
       </c>
     </row>
     <row r="7" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A7" s="10" t="s">
+      <c r="A7" s="9" t="s">
         <v>96</v>
       </c>
       <c r="B7" t="s">
@@ -873,7 +878,7 @@
       </c>
     </row>
     <row r="8" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A8" s="10" t="s">
+      <c r="A8" s="9" t="s">
         <v>108</v>
       </c>
       <c r="B8" t="s">
@@ -881,7 +886,7 @@
       </c>
     </row>
     <row r="9" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A9" s="10" t="s">
+      <c r="A9" s="9" t="s">
         <v>111</v>
       </c>
       <c r="B9" t="s">
@@ -1017,7 +1022,7 @@
       </c>
     </row>
     <row r="26" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A26" s="8" t="s">
+      <c r="A26" t="s">
         <v>61</v>
       </c>
       <c r="B26" t="s">
@@ -1033,7 +1038,7 @@
       </c>
     </row>
     <row r="28" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A28" s="8" t="s">
+      <c r="A28" t="s">
         <v>20</v>
       </c>
       <c r="B28" t="s">
@@ -1137,7 +1142,7 @@
       </c>
     </row>
     <row r="41" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A41" s="9" t="s">
+      <c r="A41" s="8" t="s">
         <v>77</v>
       </c>
       <c r="B41" t="s">
@@ -1233,7 +1238,7 @@
       </c>
     </row>
     <row r="53" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A53" s="5" t="s">
+      <c r="A53" s="11" t="s">
         <v>83</v>
       </c>
       <c r="B53" t="s">
@@ -1249,7 +1254,7 @@
       </c>
     </row>
     <row r="55" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A55" s="11" t="s">
+      <c r="A55" s="10" t="s">
         <v>88</v>
       </c>
       <c r="B55" t="s">
@@ -1265,7 +1270,7 @@
       </c>
     </row>
     <row r="57" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A57" s="11" t="s">
+      <c r="A57" s="10" t="s">
         <v>104</v>
       </c>
       <c r="B57" t="s">
@@ -1281,7 +1286,7 @@
       </c>
     </row>
     <row r="59" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A59" s="8" t="s">
+      <c r="A59" t="s">
         <v>38</v>
       </c>
       <c r="B59" t="s">
@@ -1289,7 +1294,7 @@
       </c>
     </row>
     <row r="60" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A60" s="8" t="s">
+      <c r="A60" t="s">
         <v>39</v>
       </c>
       <c r="B60" t="s">
@@ -1297,7 +1302,7 @@
       </c>
     </row>
     <row r="61" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A61" s="8" t="s">
+      <c r="A61" t="s">
         <v>45</v>
       </c>
       <c r="B61" t="s">
@@ -1305,7 +1310,7 @@
       </c>
     </row>
     <row r="62" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A62" s="8" t="s">
+      <c r="A62" t="s">
         <v>46</v>
       </c>
       <c r="B62" t="s">
@@ -1329,7 +1334,7 @@
       </c>
     </row>
     <row r="65" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A65" s="8" t="s">
+      <c r="A65" t="s">
         <v>48</v>
       </c>
       <c r="B65" t="s">
@@ -1345,7 +1350,7 @@
       </c>
     </row>
     <row r="67" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A67" s="8" t="s">
+      <c r="A67" t="s">
         <v>50</v>
       </c>
       <c r="B67" t="s">
@@ -1441,7 +1446,7 @@
       </c>
     </row>
     <row r="79" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A79" s="8" t="s">
+      <c r="A79" t="s">
         <v>40</v>
       </c>
       <c r="B79" t="s">
@@ -1457,7 +1462,7 @@
       </c>
     </row>
     <row r="81" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A81" s="8" t="s">
+      <c r="A81" t="s">
         <v>53</v>
       </c>
       <c r="B81" t="s">
@@ -1633,7 +1638,7 @@
       </c>
     </row>
     <row r="103" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A103" s="5" t="s">
+      <c r="A103" s="11" t="s">
         <v>114</v>
       </c>
       <c r="B103" t="s">
@@ -1656,9 +1661,20 @@
         <v>68</v>
       </c>
     </row>
+    <row r="106" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A106" s="5" t="s">
+        <v>117</v>
+      </c>
+      <c r="B106" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="107" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A107" s="5"/>
+    </row>
   </sheetData>
   <autoFilter ref="A1:B57" xr:uid="{904F3AA4-01F5-4399-A1EE-4BB38BAA3B9E}">
-    <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:B101">
+    <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:B106">
       <sortCondition ref="B1:B57"/>
     </sortState>
   </autoFilter>

</xml_diff>